<commit_message>
Add reference data and spread sheets
</commit_message>
<xml_diff>
--- a/Banking_Mobile_Application_Usage_Analysis_ETL_Data_App_Not_Use.xlsx
+++ b/Banking_Mobile_Application_Usage_Analysis_ETL_Data_App_Not_Use.xlsx
@@ -8,19 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\MSC\3RD-SEM\CS5651 - Statistical Inference\UOM_2020_CS5651_Statistical_Inference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE17CCC-3F57-4531-98B6-0EB0768EA862}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1D6D0E-F500-42B0-A4DA-EEEC3E299516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-4755" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Banking_Mobile_Application_Usag" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Banking_Mobile_Application_Usag!$G$2:$G$49</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="0">Banking_Mobile_Application_Usag!#REF!</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="129">
   <si>
     <t>ID</t>
   </si>
@@ -380,13 +387,40 @@
   </si>
   <si>
     <t>2020/11/16 7:16:09 AM GMT+5:30</t>
+  </si>
+  <si>
+    <t>Employment Status</t>
+  </si>
+  <si>
+    <t>No. of Participant</t>
+  </si>
+  <si>
+    <t>IN_USE</t>
+  </si>
+  <si>
+    <t>NOT_IN_USE</t>
+  </si>
+  <si>
+    <t> Category</t>
+  </si>
+  <si>
+    <t>App In Use</t>
+  </si>
+  <si>
+    <t>App Not In Use</t>
+  </si>
+  <si>
+    <t>GOVERNMENT_AND_OTHER</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,6 +560,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -709,7 +756,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -824,6 +871,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF202020"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF202020"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF202020"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF202020"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -869,10 +931,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1228,18 +1299,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE49"/>
+  <dimension ref="A1:AE65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AE1" sqref="A1:AE1"/>
+    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
@@ -5923,8 +5994,458 @@
         <v>101</v>
       </c>
     </row>
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>120</v>
+      </c>
+      <c r="C53" t="s">
+        <v>121</v>
+      </c>
+      <c r="F53" t="s">
+        <v>120</v>
+      </c>
+      <c r="G53" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>35</v>
+      </c>
+      <c r="C54">
+        <f>COUNTIF($G$2:$G$49,$B54)</f>
+        <v>16</v>
+      </c>
+      <c r="F54" t="s">
+        <v>35</v>
+      </c>
+      <c r="G54">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>46</v>
+      </c>
+      <c r="C55">
+        <f t="shared" ref="C55:C58" si="0">COUNTIF($G$2:$G$49,$B55)</f>
+        <v>26</v>
+      </c>
+      <c r="F55" t="s">
+        <v>46</v>
+      </c>
+      <c r="G55">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>53</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F56" t="s">
+        <v>53</v>
+      </c>
+      <c r="G56">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F57" t="s">
+        <v>72</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>84</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F58" t="s">
+        <v>84</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>122</v>
+      </c>
+      <c r="D60" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61">
+        <v>67</v>
+      </c>
+      <c r="D61">
+        <f>COUNTIF($G$2:$G$49,$B61)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>46</v>
+      </c>
+      <c r="C62">
+        <v>24</v>
+      </c>
+      <c r="D62">
+        <f t="shared" ref="D62:D65" si="1">COUNTIF($G$2:$G$49,$B62)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>53</v>
+      </c>
+      <c r="C63">
+        <v>10</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>72</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>84</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00954A0-0F02-4075-99F1-FD11ED88717F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70672DC-BE60-4110-B1F0-3139BB3FCD69}">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2">
+        <v>67</v>
+      </c>
+      <c r="C2">
+        <v>16</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="5">
+        <v>67</v>
+      </c>
+      <c r="K2" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="57.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>26</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="J3" s="5">
+        <v>36</v>
+      </c>
+      <c r="K3" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <f>SUM(B3:B6)</f>
+        <v>36</v>
+      </c>
+      <c r="F4">
+        <f>SUM(C3:C6)</f>
+        <v>32</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J4" s="5">
+        <f>SUM(J2:J3)</f>
+        <v>103</v>
+      </c>
+      <c r="K4" s="5">
+        <f>SUM(K2:K3)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>SUM(B2:B6)</f>
+        <v>103</v>
+      </c>
+      <c r="C7">
+        <f>SUM(C2:C6)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>67</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>SUM(B11:B14)</f>
+        <v>36</v>
+      </c>
+      <c r="C16">
+        <f>SUM(C11:C14)</f>
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF80182-45C0-4C1F-B582-88815B40DCE8}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="5">
+        <v>67</v>
+      </c>
+      <c r="C2" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="5">
+        <v>36</v>
+      </c>
+      <c r="C3" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="5">
+        <f>SUM(B2:B3)</f>
+        <v>103</v>
+      </c>
+      <c r="C4" s="5">
+        <f>SUM(C2:C3)</f>
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>